<commit_message>
smooth interpolation of SIMTRA profiles. analytycal integration of 1-st order interpolants
</commit_message>
<xml_diff>
--- a/saves/simtra.xlsx
+++ b/saves/simtra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Георгий\Desktop\ФТИ\RotationAndDeposition\saves\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\ФТИ\RotationAndDeposition\saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD09A90E-4290-4285-A1D1-4F72378676BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063F34A8-1F54-4635-BCE4-8B423EA58F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="150">
   <si>
     <t>Способ задания профиля распыления</t>
   </si>
@@ -464,6 +464,12 @@
   </si>
   <si>
     <t>saves\N.txt</t>
+  </si>
+  <si>
+    <t>Сглаживание профиля</t>
+  </si>
+  <si>
+    <t>smooth</t>
   </si>
 </sst>
 </file>
@@ -526,7 +532,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -826,18 +832,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="92.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="92.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -866,7 +872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>0</v>
       </c>
@@ -889,7 +895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
@@ -915,7 +921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
@@ -941,7 +947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>3</v>
       </c>
@@ -967,7 +973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>4</v>
       </c>
@@ -993,7 +999,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1045,7 +1051,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1097,7 +1103,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1166,7 +1172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1192,7 +1198,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1221,7 +1227,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1250,7 +1256,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1276,7 +1282,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1299,7 +1305,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1322,7 +1328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1371,7 +1377,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1400,7 +1406,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1423,7 +1429,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1446,7 +1452,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1469,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1492,7 +1498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1515,7 +1521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1541,7 +1547,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1593,7 +1599,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1616,7 +1622,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1639,7 +1645,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1662,7 +1668,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1763,7 +1769,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1835,7 +1841,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1916,7 +1922,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1942,7 +1948,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1966,6 +1972,26 @@
       </c>
       <c r="I45" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>139</v>
+      </c>
+      <c r="G46" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>